<commit_message>
Fixed proc Use and Modify
</commit_message>
<xml_diff>
--- a/Tests09/Sample-Queries-7-Line numbers.xlsx
+++ b/Tests09/Sample-Queries-7-Line numbers.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitigator\Documents\CS3201-2-Group-9-SPA\Tests09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\limji\Desktop\Coding Projects\CS3201-2-Group-9-SPA\Tests09\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="3264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -452,7 +452,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -763,21 +763,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="B216" sqref="B216:B226"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="R223" sqref="R223"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -793,7 +793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -801,7 +801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -809,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -817,7 +817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -825,7 +825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -833,7 +833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -841,7 +841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -849,7 +849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -857,7 +857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -865,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -873,17 +873,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -891,12 +891,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -904,7 +904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
@@ -912,17 +912,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>16</v>
       </c>
@@ -930,7 +930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>12</v>
       </c>
@@ -939,7 +939,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>17</v>
       </c>
@@ -951,7 +951,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>18</v>
       </c>
@@ -963,7 +963,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>12</v>
       </c>
@@ -972,7 +972,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>19</v>
       </c>
@@ -980,7 +980,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>20</v>
       </c>
@@ -988,7 +988,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>21</v>
       </c>
@@ -996,7 +996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>22</v>
       </c>
@@ -1004,12 +1004,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>23</v>
       </c>
@@ -1017,17 +1017,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>24</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>25</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>26</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>27</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>28</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E40" t="s">
         <v>29</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E41" t="s">
         <v>13</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>29</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>30</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
         <v>12</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>31</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>32</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>33</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>34</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F49" t="s">
         <v>29</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
         <v>13</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>35</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F52" t="s">
         <v>12</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>36</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E54" t="s">
         <v>12</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>37</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>38</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
         <v>12</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>13</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>39</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>40</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
         <v>29</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
         <v>12</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
         <v>13</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>41</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
         <v>12</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>12</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>43</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>42</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>43</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>44</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>45</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>46</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>47</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>48</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E75" t="s">
         <v>29</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E76" t="s">
         <v>13</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>49</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E78" t="s">
         <v>12</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>50</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>51</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>52</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>53</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>54</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>55</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H85" t="s">
         <v>12</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G86" t="s">
         <v>12</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>56</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>57</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>58</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F90" t="s">
         <v>29</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F91" t="s">
         <v>13</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>59</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F93" t="s">
         <v>12</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>60</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>61</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E96" t="s">
         <v>12</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
         <v>12</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C98" t="s">
         <v>29</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C99" t="s">
         <v>13</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>62</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>63</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>64</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D103" t="s">
         <v>29</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D104" t="s">
         <v>13</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>65</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>66</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E107" t="s">
         <v>68</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>67</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E109" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D110" t="s">
         <v>12</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
         <v>12</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>68</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>69</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>70</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>12</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>73</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>71</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>72</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>73</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>74</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>75</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D122" t="s">
         <v>29</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D123" t="s">
         <v>13</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>76</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>77</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>78</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E127" t="s">
         <v>29</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E128" t="s">
         <v>13</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>79</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>80</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E131" t="s">
         <v>12</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D132" t="s">
         <v>12</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>81</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>82</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C135" t="s">
         <v>12</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>83</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>12</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>87</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>84</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>85</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>86</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>87</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>88</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>89</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E145" t="s">
         <v>12</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>90</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>91</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>92</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>93</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F150" t="s">
         <v>29</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F151" t="s">
         <v>13</v>
       </c>
@@ -2286,9 +2286,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G152" t="s">
         <v>98</v>
@@ -2298,7 +2298,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F153" t="s">
         <v>12</v>
       </c>
@@ -2307,9 +2307,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F154" t="s">
         <v>99</v>
@@ -2319,7 +2319,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E155" t="s">
         <v>12</v>
       </c>
@@ -2328,9 +2328,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E156" t="s">
         <v>100</v>
@@ -2340,9 +2340,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E157" t="s">
         <v>101</v>
@@ -2352,9 +2352,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E158" t="s">
         <v>102</v>
@@ -2364,7 +2364,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D159" t="s">
         <v>12</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C160" t="s">
         <v>12</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
         <v>12</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
         <v>103</v>
       </c>
@@ -2400,9 +2400,9 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C163" t="s">
         <v>5</v>
@@ -2412,9 +2412,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C164" t="s">
         <v>104</v>
@@ -2424,9 +2424,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D165" t="s">
         <v>105</v>
@@ -2436,9 +2436,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D166" t="s">
         <v>106</v>
@@ -2448,9 +2448,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E167" t="s">
         <v>107</v>
@@ -2460,7 +2460,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D168" t="s">
         <v>12</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D169" t="s">
         <v>13</v>
       </c>
@@ -2478,9 +2478,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E170" t="s">
         <v>108</v>
@@ -2490,7 +2490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D171" t="s">
         <v>12</v>
       </c>
@@ -2499,9 +2499,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D172" t="s">
         <v>94</v>
@@ -2511,9 +2511,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E173" t="s">
         <v>109</v>
@@ -2523,7 +2523,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D174" t="s">
         <v>12</v>
       </c>
@@ -2532,9 +2532,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D175" t="s">
         <v>110</v>
@@ -2544,7 +2544,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C176" t="s">
         <v>12</v>
       </c>
@@ -2553,9 +2553,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C177" t="s">
         <v>111</v>
@@ -2565,9 +2565,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D178" t="s">
         <v>112</v>
@@ -2577,7 +2577,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C179" t="s">
         <v>68</v>
       </c>
@@ -2586,9 +2586,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D180" t="s">
         <v>113</v>
@@ -2598,9 +2598,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D181" t="s">
         <v>114</v>
@@ -2610,7 +2610,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C182" t="s">
         <v>12</v>
       </c>
@@ -2619,9 +2619,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C183" t="s">
         <v>95</v>
@@ -2631,9 +2631,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D184" t="s">
         <v>115</v>
@@ -2643,9 +2643,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D185" t="s">
         <v>116</v>
@@ -2655,7 +2655,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C186" t="s">
         <v>68</v>
       </c>
@@ -2664,9 +2664,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D187" t="s">
         <v>97</v>
@@ -2676,7 +2676,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C188" t="s">
         <v>12</v>
       </c>
@@ -2685,9 +2685,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C189" t="s">
         <v>117</v>
@@ -2697,9 +2697,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C190" t="s">
         <v>118</v>
@@ -2709,7 +2709,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
         <v>12</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B192" t="s">
         <v>119</v>
       </c>
@@ -2727,9 +2727,9 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C193" t="s">
         <v>120</v>
@@ -2739,9 +2739,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C194" t="s">
         <v>5</v>
@@ -2751,9 +2751,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C195" t="s">
         <v>121</v>
@@ -2763,9 +2763,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C196" t="s">
         <v>122</v>
@@ -2775,9 +2775,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D197" t="s">
         <v>18</v>
@@ -2787,7 +2787,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C198" t="s">
         <v>29</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C199" t="s">
         <v>13</v>
       </c>
@@ -2805,9 +2805,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D200" t="s">
         <v>76</v>
@@ -2817,9 +2817,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E201" t="s">
         <v>18</v>
@@ -2829,7 +2829,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D202" t="s">
         <v>12</v>
       </c>
@@ -2838,9 +2838,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D203" t="s">
         <v>5</v>
@@ -2850,7 +2850,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C204" t="s">
         <v>12</v>
       </c>
@@ -2859,9 +2859,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C205" t="s">
         <v>123</v>
@@ -2871,9 +2871,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D206" t="s">
         <v>124</v>
@@ -2883,9 +2883,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D207" t="s">
         <v>125</v>
@@ -2895,7 +2895,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C208" t="s">
         <v>29</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C209" t="s">
         <v>13</v>
       </c>
@@ -2913,9 +2913,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D210" t="s">
         <v>65</v>
@@ -2925,7 +2925,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C211" t="s">
         <v>12</v>
       </c>
@@ -2934,9 +2934,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A212">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C212" t="s">
         <v>126</v>
@@ -2946,9 +2946,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A213">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C213" t="s">
         <v>127</v>
@@ -2958,7 +2958,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B214" t="s">
         <v>12</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B215" t="s">
         <v>128</v>
       </c>
@@ -2976,9 +2976,9 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C216" t="s">
         <v>129</v>
@@ -2988,9 +2988,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C217" t="s">
         <v>130</v>
@@ -3000,9 +3000,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C218" t="s">
         <v>131</v>
@@ -3012,9 +3012,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A219">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C219" t="s">
         <v>132</v>
@@ -3024,9 +3024,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C220" t="s">
         <v>133</v>
@@ -3036,9 +3036,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A221">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C221" t="s">
         <v>134</v>
@@ -3048,9 +3048,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A222">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C222" t="s">
         <v>135</v>
@@ -3060,9 +3060,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A223">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C223" t="s">
         <v>136</v>
@@ -3072,9 +3072,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C224" t="s">
         <v>137</v>
@@ -3084,9 +3084,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C225" t="s">
         <v>138</v>
@@ -3096,9 +3096,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C226" t="s">
         <v>139</v>
@@ -3108,7 +3108,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B227" t="s">
         <v>12</v>
       </c>

</xml_diff>